<commit_message>
There is a bug. When you overwrite a selection it erases all the other choices. No located yet where the bug originates.
</commit_message>
<xml_diff>
--- a/Data/Source recepten.xlsx
+++ b/Data/Source recepten.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$76</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$88</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="140">
   <si>
     <t xml:space="preserve">Cuisine</t>
   </si>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Advocado met spek en peultjes</t>
   </si>
   <si>
-    <t xml:space="preserve">Advocado</t>
+    <t xml:space="preserve">Avocado</t>
   </si>
   <si>
     <t xml:space="preserve">Peultjes</t>
@@ -293,6 +293,156 @@
   </si>
   <si>
     <t xml:space="preserve">Limoen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tortilla Met Chorizo en Ui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheddar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chorizo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rode Paprika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groene Chilipeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huevos Rancheros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Komijn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gehakt met Bloemkool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoete Paprika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosbief met Parmezaan en Avocado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosbief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parmezaan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm Gerookte Zalm met Groenten en Citroendip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm Gerookte Zalm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viswinkel of Cru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groene Asperges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspergebroccoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verse Room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eetlepels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonijnpizza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonijn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psylliumvezels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bio Planet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomatensaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ontpitte Olijven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gedroogde Oregano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teelepels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chilizalm met Koriandercreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zalmfilet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harissa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayonaise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verse Muntblaadjes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kip met Speksaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spek in dunne plakjes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broccoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kipshoarma met Bloemkoolrijst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rode Chilipeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Garam Masala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomatenpuree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fijngehakte Amandelen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duivelse Kip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roomkaas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slagroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingelegde Jalapeno’s</t>
   </si>
 </sst>
 </file>
@@ -407,25 +557,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E90" activeCellId="0" sqref="E90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A119" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K150" activeCellId="0" sqref="K150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,7 +605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -506,7 +657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
@@ -532,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
@@ -558,7 +709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
@@ -584,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>8</v>
       </c>
@@ -610,7 +761,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>8</v>
       </c>
@@ -636,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>8</v>
       </c>
@@ -662,7 +813,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>8</v>
       </c>
@@ -688,7 +839,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>8</v>
       </c>
@@ -714,7 +865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>8</v>
       </c>
@@ -740,7 +891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>8</v>
       </c>
@@ -766,7 +917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>8</v>
       </c>
@@ -792,7 +943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>8</v>
       </c>
@@ -818,7 +969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>8</v>
       </c>
@@ -844,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>8</v>
       </c>
@@ -870,7 +1021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>8</v>
       </c>
@@ -896,7 +1047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>8</v>
       </c>
@@ -922,7 +1073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>8</v>
       </c>
@@ -948,7 +1099,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>8</v>
       </c>
@@ -974,7 +1125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>8</v>
       </c>
@@ -1000,7 +1151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>8</v>
       </c>
@@ -1026,7 +1177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>8</v>
       </c>
@@ -1052,7 +1203,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>8</v>
       </c>
@@ -1078,7 +1229,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>8</v>
       </c>
@@ -1104,7 +1255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1281,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>8</v>
       </c>
@@ -1156,7 +1307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>8</v>
       </c>
@@ -1182,7 +1333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1359,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>8</v>
       </c>
@@ -1234,7 +1385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>8</v>
       </c>
@@ -1260,7 +1411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>8</v>
       </c>
@@ -1312,7 +1463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>8</v>
       </c>
@@ -1338,7 +1489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>8</v>
       </c>
@@ -1364,7 +1515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>8</v>
       </c>
@@ -1390,7 +1541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>8</v>
       </c>
@@ -1416,7 +1567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>8</v>
       </c>
@@ -1442,7 +1593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>8</v>
       </c>
@@ -1468,7 +1619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>8</v>
       </c>
@@ -1494,7 +1645,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>8</v>
       </c>
@@ -1520,7 +1671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>8</v>
       </c>
@@ -1546,7 +1697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>8</v>
       </c>
@@ -1598,7 +1749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>8</v>
       </c>
@@ -1624,7 +1775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>8</v>
       </c>
@@ -1632,7 +1783,7 @@
         <v>60</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>61</v>
@@ -1650,7 +1801,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>8</v>
       </c>
@@ -1658,7 +1809,7 @@
         <v>60</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>61</v>
@@ -1676,7 +1827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>8</v>
       </c>
@@ -1684,7 +1835,7 @@
         <v>60</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>61</v>
@@ -1702,7 +1853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>8</v>
       </c>
@@ -1710,7 +1861,7 @@
         <v>60</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>61</v>
@@ -1728,7 +1879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>8</v>
       </c>
@@ -1736,7 +1887,7 @@
         <v>60</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>61</v>
@@ -1754,7 +1905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>8</v>
       </c>
@@ -1780,7 +1931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>8</v>
       </c>
@@ -1806,7 +1957,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>8</v>
       </c>
@@ -1832,7 +1983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>8</v>
       </c>
@@ -1858,7 +2009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>8</v>
       </c>
@@ -1884,7 +2035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>8</v>
       </c>
@@ -1910,7 +2061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>8</v>
       </c>
@@ -1936,7 +2087,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>8</v>
       </c>
@@ -1956,13 +2107,13 @@
         <v>2</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="H59" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>8</v>
       </c>
@@ -1988,7 +2139,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>8</v>
       </c>
@@ -2014,7 +2165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>8</v>
       </c>
@@ -2040,7 +2191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>8</v>
       </c>
@@ -2066,7 +2217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>8</v>
       </c>
@@ -2092,7 +2243,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>8</v>
       </c>
@@ -2118,7 +2269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>8</v>
       </c>
@@ -2144,7 +2295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>8</v>
       </c>
@@ -2170,7 +2321,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>8</v>
       </c>
@@ -2196,7 +2347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>8</v>
       </c>
@@ -2222,7 +2373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>8</v>
       </c>
@@ -2248,7 +2399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>8</v>
       </c>
@@ -2274,7 +2425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>8</v>
       </c>
@@ -2300,7 +2451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>8</v>
       </c>
@@ -2326,7 +2477,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>8</v>
       </c>
@@ -2352,7 +2503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>8</v>
       </c>
@@ -2378,7 +2529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>8</v>
       </c>
@@ -2404,14 +2555,2062 @@
         <v>12</v>
       </c>
     </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H84" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H90" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H91" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H92" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H93" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H94" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H95" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G96" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H97" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="G98" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H98" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H99" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F100" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="G100" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H100" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F101" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H101" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F102" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G102" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H102" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F103" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G103" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H103" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F104" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H104" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G105" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H105" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F106" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="G106" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H106" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H107" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G108" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H108" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E109" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F109" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G109" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H109" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E110" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G110" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H110" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F111" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G111" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="H111" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F112" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G112" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H112" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E113" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F113" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G113" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H113" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E114" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G114" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H114" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G115" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H115" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="G116" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H116" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G117" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H117" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G118" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="H118" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G119" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H119" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G120" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H120" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="G121" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H121" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F122" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G122" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H122" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F123" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G123" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="H123" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E124" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G124" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H124" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E125" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F125" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G125" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H125" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E126" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F126" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G126" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H126" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D127" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F127" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G127" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H127" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F128" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G128" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H128" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F129" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G129" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H129" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F130" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G130" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H130" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F131" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="G131" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H131" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="D132" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E132" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F132" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="G132" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H132" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F133" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G133" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H133" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="D134" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E134" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F134" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G134" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H134" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="D135" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E135" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F135" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G135" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="H135" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="D136" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E136" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F136" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G136" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H136" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="D137" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E137" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F137" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="G137" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H137" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D138" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E138" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F138" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="G138" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H138" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D139" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E139" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F139" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G139" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H139" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D140" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E140" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F140" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G140" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H140" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D141" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E141" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="F141" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G141" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H141" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D142" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E142" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="F142" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G142" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H142" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D143" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E143" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F143" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G143" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H143" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D144" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E144" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F144" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G144" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H144" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D145" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E145" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F145" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="G145" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H145" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D146" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E146" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F146" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G146" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H146" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D147" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E147" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F147" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G147" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H147" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D148" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E148" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="G148" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H148" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D149" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E149" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G149" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H149" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D150" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E150" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G150" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H150" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D151" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E151" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F151" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G151" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H151" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D152" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E152" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="F152" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G152" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H152" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D153" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E153" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G153" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H153" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D154" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E154" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F154" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G154" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H154" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D155" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E155" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G155" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H155" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H76">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Bloemkool"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H88"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Corrected mistakes in the masterdata
</commit_message>
<xml_diff>
--- a/Data/Source recepten.xlsx
+++ b/Data/Source recepten.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$88</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$160</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="151">
   <si>
     <t xml:space="preserve">Cuisine</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">Gehakt met Bloemkool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gemalen Kaas</t>
   </si>
   <si>
     <t xml:space="preserve">Zoete Paprika</t>
@@ -590,13 +593,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I159"/>
+  <dimension ref="A1:I160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A114" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I160" activeCellId="0" sqref="I160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.31"/>
@@ -2720,7 +2723,7 @@
         <v>12</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="I73" s="0" t="s">
         <v>17</v>
@@ -3468,16 +3471,16 @@
         <v>106</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H99" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3494,13 +3497,13 @@
         <v>105</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H100" s="0" t="s">
         <v>13</v>
@@ -3523,13 +3526,13 @@
         <v>105</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="F101" s="0" t="n">
-        <v>2</v>
+        <v>250</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H101" s="0" t="s">
         <v>13</v>
@@ -3543,28 +3546,28 @@
         <v>9</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H102" s="0" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3578,22 +3581,22 @@
         <v>87</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H103" s="0" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3607,16 +3610,16 @@
         <v>87</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H104" s="0" t="s">
         <v>13</v>
@@ -3636,10 +3639,10 @@
         <v>87</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="F105" s="0" t="n">
         <v>100</v>
@@ -3651,7 +3654,7 @@
         <v>13</v>
       </c>
       <c r="I105" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,25 +3665,25 @@
         <v>78</v>
       </c>
       <c r="C106" s="0" t="n">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D106" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="E106" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="E106" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="F106" s="0" t="n">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="G106" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H106" s="0" t="s">
-        <v>112</v>
+        <v>13</v>
       </c>
       <c r="I106" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,22 +3697,22 @@
         <v>96</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E107" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H107" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="F107" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G107" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H107" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="I107" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3723,16 +3726,16 @@
         <v>96</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E108" s="0" t="s">
         <v>114</v>
       </c>
       <c r="F108" s="0" t="n">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H108" s="0" t="s">
         <v>13</v>
@@ -3752,22 +3755,22 @@
         <v>96</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E109" s="0" t="s">
         <v>115</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>3</v>
+        <v>400</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="H109" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3781,22 +3784,22 @@
         <v>96</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="H110" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I110" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3807,25 +3810,25 @@
         <v>78</v>
       </c>
       <c r="C111" s="0" t="n">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="H111" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I111" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,22 +3842,22 @@
         <v>99</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="F112" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="H112" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I112" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3868,22 +3871,22 @@
         <v>99</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>120</v>
+        <v>31</v>
       </c>
       <c r="F113" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="H113" s="0" t="s">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="I113" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3897,19 +3900,19 @@
         <v>99</v>
       </c>
       <c r="D114" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E114" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G114" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="E114" s="0" t="s">
+      <c r="H114" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="F114" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G114" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H114" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="I114" s="0" t="s">
         <v>24</v>
@@ -3926,10 +3929,10 @@
         <v>99</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="F115" s="0" t="n">
         <v>100</v>
@@ -3941,7 +3944,7 @@
         <v>13</v>
       </c>
       <c r="I115" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3955,13 +3958,13 @@
         <v>99</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="F116" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G116" s="0" t="s">
         <v>16</v>
@@ -3970,7 +3973,7 @@
         <v>13</v>
       </c>
       <c r="I116" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3984,13 +3987,13 @@
         <v>99</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G117" s="0" t="s">
         <v>16</v>
@@ -3999,7 +4002,7 @@
         <v>13</v>
       </c>
       <c r="I117" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4013,16 +4016,16 @@
         <v>99</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E118" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F118" s="0" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G118" s="0" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="H118" s="0" t="s">
         <v>13</v>
@@ -4042,16 +4045,16 @@
         <v>99</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E119" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G119" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="F119" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G119" s="0" t="s">
-        <v>116</v>
       </c>
       <c r="H119" s="0" t="s">
         <v>13</v>
@@ -4071,22 +4074,22 @@
         <v>99</v>
       </c>
       <c r="D120" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G120" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="E120" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F120" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G120" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="H120" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I120" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4097,25 +4100,25 @@
         <v>78</v>
       </c>
       <c r="C121" s="0" t="n">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="F121" s="0" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="G121" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H121" s="0" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="I121" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4129,22 +4132,22 @@
         <v>133</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="G122" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H122" s="0" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="I122" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4158,22 +4161,22 @@
         <v>133</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="F123" s="0" t="n">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="G123" s="0" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="H123" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I123" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,22 +4190,22 @@
         <v>133</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F124" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G124" s="0" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="H124" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I124" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4216,16 +4219,16 @@
         <v>133</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="F125" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="H125" s="0" t="s">
         <v>13</v>
@@ -4245,22 +4248,22 @@
         <v>133</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G126" s="0" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="H126" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I126" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4274,16 +4277,16 @@
         <v>133</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H127" s="0" t="s">
         <v>13</v>
@@ -4303,22 +4306,22 @@
         <v>133</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E128" s="0" t="s">
         <v>131</v>
       </c>
       <c r="F128" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G128" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H128" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I128" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4332,16 +4335,16 @@
         <v>133</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G129" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H129" s="0" t="s">
         <v>13</v>
@@ -4361,16 +4364,16 @@
         <v>133</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="G130" s="0" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="H130" s="0" t="s">
         <v>13</v>
@@ -4390,13 +4393,13 @@
         <v>133</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>140</v>
+        <v>400</v>
       </c>
       <c r="G131" s="0" t="s">
         <v>16</v>
@@ -4416,16 +4419,16 @@
         <v>78</v>
       </c>
       <c r="C132" s="0" t="n">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="F132" s="0" t="n">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="G132" s="0" t="s">
         <v>16</v>
@@ -4434,7 +4437,7 @@
         <v>13</v>
       </c>
       <c r="I132" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4448,13 +4451,13 @@
         <v>142</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="G133" s="0" t="s">
         <v>16</v>
@@ -4463,7 +4466,7 @@
         <v>13</v>
       </c>
       <c r="I133" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4477,10 +4480,10 @@
         <v>142</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="F134" s="0" t="n">
         <v>50</v>
@@ -4492,7 +4495,7 @@
         <v>13</v>
       </c>
       <c r="I134" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,22 +4509,22 @@
         <v>142</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="F135" s="0" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="G135" s="0" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="H135" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I135" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4535,16 +4538,16 @@
         <v>142</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F136" s="0" t="n">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="G136" s="0" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="H136" s="0" t="s">
         <v>13</v>
@@ -4564,13 +4567,13 @@
         <v>142</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="G137" s="0" t="s">
         <v>16</v>
@@ -4579,7 +4582,7 @@
         <v>13</v>
       </c>
       <c r="I137" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4590,16 +4593,16 @@
         <v>78</v>
       </c>
       <c r="C138" s="0" t="n">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D138" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E138" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="E138" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="F138" s="0" t="n">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="G138" s="0" t="s">
         <v>16</v>
@@ -4608,7 +4611,7 @@
         <v>13</v>
       </c>
       <c r="I138" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4622,22 +4625,22 @@
         <v>147</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E139" s="0" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F139" s="0" t="n">
-        <v>1</v>
+        <v>280</v>
       </c>
       <c r="G139" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H139" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I139" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4651,16 +4654,16 @@
         <v>147</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="F140" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G140" s="0" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="H140" s="0" t="s">
         <v>13</v>
@@ -4680,16 +4683,16 @@
         <v>147</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="F141" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G141" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="H141" s="0" t="s">
         <v>13</v>
@@ -4709,13 +4712,13 @@
         <v>147</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E142" s="0" t="s">
         <v>138</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G142" s="0" t="s">
         <v>16</v>
@@ -4738,22 +4741,22 @@
         <v>147</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E143" s="0" t="s">
         <v>139</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G143" s="0" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="H143" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I143" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4767,7 +4770,7 @@
         <v>147</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E144" s="0" t="s">
         <v>140</v>
@@ -4776,7 +4779,7 @@
         <v>1</v>
       </c>
       <c r="G144" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H144" s="0" t="s">
         <v>13</v>
@@ -4796,22 +4799,22 @@
         <v>147</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="F145" s="0" t="n">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="G145" s="0" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="H145" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I145" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4825,22 +4828,22 @@
         <v>147</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>5</v>
+        <v>300</v>
       </c>
       <c r="G146" s="0" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="H146" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I146" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4854,22 +4857,22 @@
         <v>147</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G147" s="0" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="H147" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I147" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4880,16 +4883,16 @@
         <v>78</v>
       </c>
       <c r="C148" s="0" t="n">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D148" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E148" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E148" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="F148" s="0" t="n">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G148" s="0" t="s">
         <v>16</v>
@@ -4898,7 +4901,7 @@
         <v>13</v>
       </c>
       <c r="I148" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4912,13 +4915,13 @@
         <v>148</v>
       </c>
       <c r="D149" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E149" s="0" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>30</v>
+        <v>280</v>
       </c>
       <c r="G149" s="0" t="s">
         <v>16</v>
@@ -4927,7 +4930,7 @@
         <v>13</v>
       </c>
       <c r="I149" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4941,16 +4944,16 @@
         <v>148</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E150" s="0" t="s">
         <v>144</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G150" s="0" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="H150" s="0" t="s">
         <v>13</v>
@@ -4970,22 +4973,22 @@
         <v>148</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="G151" s="0" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="H151" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I151" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4999,16 +5002,16 @@
         <v>148</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="F152" s="0" t="n">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="G152" s="0" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="H152" s="0" t="s">
         <v>13</v>
@@ -5028,22 +5031,22 @@
         <v>148</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E153" s="0" t="s">
-        <v>15</v>
+        <v>146</v>
       </c>
       <c r="F153" s="0" t="n">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="G153" s="0" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="H153" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I153" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5057,13 +5060,13 @@
         <v>148</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>97</v>
+        <v>15</v>
       </c>
       <c r="F154" s="0" t="n">
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="G154" s="0" t="s">
         <v>16</v>
@@ -5072,7 +5075,7 @@
         <v>13</v>
       </c>
       <c r="I154" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5086,22 +5089,22 @@
         <v>148</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F155" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="G155" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H155" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I155" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5109,28 +5112,28 @@
         <v>9</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C156" s="0" t="n">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="F156" s="0" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G156" s="0" t="s">
         <v>12</v>
       </c>
       <c r="H156" s="0" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="I156" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5144,22 +5147,22 @@
         <v>98</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E157" s="0" t="s">
         <v>148</v>
       </c>
       <c r="F157" s="0" t="n">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="G157" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H157" s="0" t="s">
         <v>81</v>
       </c>
       <c r="I157" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5173,22 +5176,22 @@
         <v>98</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E158" s="0" t="s">
         <v>149</v>
       </c>
       <c r="F158" s="0" t="n">
-        <v>80</v>
+        <v>400</v>
       </c>
       <c r="G158" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H158" s="0" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="I158" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5202,13 +5205,13 @@
         <v>98</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E159" s="0" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="F159" s="0" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="G159" s="0" t="s">
         <v>16</v>
@@ -5220,8 +5223,37 @@
         <v>24</v>
       </c>
     </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="D160" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E160" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F160" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G160" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H160" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I160" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H88"/>
+  <autoFilter ref="A1:H160"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Corrected a bug in one of the recipies
</commit_message>
<xml_diff>
--- a/Data/Source recepten.xlsx
+++ b/Data/Source recepten.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$160</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$161</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="152">
   <si>
     <t xml:space="preserve">Cuisine</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">Gehakt met Bloemkool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grote Wortelen</t>
   </si>
   <si>
     <t xml:space="preserve">Gemalen Kaas</t>
@@ -593,13 +596,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J92" activeCellId="0" sqref="J92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.31"/>
@@ -3455,9 +3458,6 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="B99" s="0" t="s">
         <v>83</v>
       </c>
@@ -3471,16 +3471,16 @@
         <v>106</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H99" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3500,16 +3500,16 @@
         <v>107</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H100" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I100" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3526,13 +3526,13 @@
         <v>105</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="F101" s="0" t="n">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H101" s="0" t="s">
         <v>13</v>
@@ -3555,13 +3555,13 @@
         <v>105</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>2</v>
+        <v>250</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H102" s="0" t="s">
         <v>13</v>
@@ -3575,28 +3575,28 @@
         <v>9</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H103" s="0" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,22 +3610,22 @@
         <v>87</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H104" s="0" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="I104" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3639,16 +3639,16 @@
         <v>87</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H105" s="0" t="s">
         <v>13</v>
@@ -3668,10 +3668,10 @@
         <v>87</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="F106" s="0" t="n">
         <v>100</v>
@@ -3683,7 +3683,7 @@
         <v>13</v>
       </c>
       <c r="I106" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,25 +3694,25 @@
         <v>78</v>
       </c>
       <c r="C107" s="0" t="n">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D107" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E107" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E107" s="0" t="s">
-        <v>112</v>
-      </c>
       <c r="F107" s="0" t="n">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="G107" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H107" s="0" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3726,22 +3726,22 @@
         <v>96</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E108" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="G108" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H108" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="F108" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G108" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H108" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="I108" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3755,16 +3755,16 @@
         <v>96</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E109" s="0" t="s">
         <v>115</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H109" s="0" t="s">
         <v>13</v>
@@ -3784,22 +3784,22 @@
         <v>96</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E110" s="0" t="s">
         <v>116</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>3</v>
+        <v>400</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="H110" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I110" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3813,22 +3813,22 @@
         <v>96</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="H111" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I111" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,25 +3839,25 @@
         <v>78</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
       <c r="F112" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="H112" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I112" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3871,22 +3871,22 @@
         <v>99</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="F113" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="H113" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I113" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3900,22 +3900,22 @@
         <v>99</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
       <c r="F114" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G114" s="0" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
       <c r="H114" s="0" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="I114" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3929,19 +3929,19 @@
         <v>99</v>
       </c>
       <c r="D115" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G115" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="E115" s="0" t="s">
+      <c r="H115" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="F115" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G115" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H115" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="I115" s="0" t="s">
         <v>24</v>
@@ -3958,10 +3958,10 @@
         <v>99</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="F116" s="0" t="n">
         <v>100</v>
@@ -3973,7 +3973,7 @@
         <v>13</v>
       </c>
       <c r="I116" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3987,13 +3987,13 @@
         <v>99</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G117" s="0" t="s">
         <v>16</v>
@@ -4002,7 +4002,7 @@
         <v>13</v>
       </c>
       <c r="I117" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4016,13 +4016,13 @@
         <v>99</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="F118" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G118" s="0" t="s">
         <v>16</v>
@@ -4031,7 +4031,7 @@
         <v>13</v>
       </c>
       <c r="I118" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4045,16 +4045,16 @@
         <v>99</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E119" s="0" t="s">
         <v>125</v>
       </c>
       <c r="F119" s="0" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="H119" s="0" t="s">
         <v>13</v>
@@ -4074,16 +4074,16 @@
         <v>99</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E120" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G120" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="F120" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G120" s="0" t="s">
-        <v>117</v>
       </c>
       <c r="H120" s="0" t="s">
         <v>13</v>
@@ -4103,22 +4103,22 @@
         <v>99</v>
       </c>
       <c r="D121" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G121" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="E121" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F121" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G121" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="H121" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I121" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4129,25 +4129,25 @@
         <v>78</v>
       </c>
       <c r="C122" s="0" t="n">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="G122" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H122" s="0" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="I122" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4161,22 +4161,22 @@
         <v>133</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="F123" s="0" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="G123" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H123" s="0" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="I123" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4190,22 +4190,22 @@
         <v>133</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="F124" s="0" t="n">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="G124" s="0" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="H124" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I124" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4219,22 +4219,22 @@
         <v>133</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="F125" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>12</v>
+        <v>127</v>
       </c>
       <c r="H125" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I125" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4248,16 +4248,16 @@
         <v>133</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G126" s="0" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="H126" s="0" t="s">
         <v>13</v>
@@ -4277,22 +4277,22 @@
         <v>133</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="H127" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I127" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4306,16 +4306,16 @@
         <v>133</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="F128" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G128" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H128" s="0" t="s">
         <v>13</v>
@@ -4335,22 +4335,22 @@
         <v>133</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E129" s="0" t="s">
         <v>132</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G129" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H129" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I129" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4364,16 +4364,16 @@
         <v>133</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G130" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H130" s="0" t="s">
         <v>13</v>
@@ -4393,16 +4393,16 @@
         <v>133</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="G131" s="0" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="H131" s="0" t="s">
         <v>13</v>
@@ -4422,13 +4422,13 @@
         <v>133</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="F132" s="0" t="n">
-        <v>140</v>
+        <v>400</v>
       </c>
       <c r="G132" s="0" t="s">
         <v>16</v>
@@ -4448,16 +4448,16 @@
         <v>78</v>
       </c>
       <c r="C133" s="0" t="n">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="G133" s="0" t="s">
         <v>16</v>
@@ -4466,7 +4466,7 @@
         <v>13</v>
       </c>
       <c r="I133" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,13 +4480,13 @@
         <v>142</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="F134" s="0" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="G134" s="0" t="s">
         <v>16</v>
@@ -4495,7 +4495,7 @@
         <v>13</v>
       </c>
       <c r="I134" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4509,10 +4509,10 @@
         <v>142</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="F135" s="0" t="n">
         <v>50</v>
@@ -4524,7 +4524,7 @@
         <v>13</v>
       </c>
       <c r="I135" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4538,22 +4538,22 @@
         <v>142</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="F136" s="0" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="G136" s="0" t="s">
-        <v>135</v>
+        <v>16</v>
       </c>
       <c r="H136" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I136" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4567,16 +4567,16 @@
         <v>142</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="G137" s="0" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="H137" s="0" t="s">
         <v>13</v>
@@ -4596,13 +4596,13 @@
         <v>142</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E138" s="0" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="F138" s="0" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="G138" s="0" t="s">
         <v>16</v>
@@ -4611,7 +4611,7 @@
         <v>13</v>
       </c>
       <c r="I138" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4622,16 +4622,16 @@
         <v>78</v>
       </c>
       <c r="C139" s="0" t="n">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D139" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E139" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="E139" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="F139" s="0" t="n">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="G139" s="0" t="s">
         <v>16</v>
@@ -4640,7 +4640,7 @@
         <v>13</v>
       </c>
       <c r="I139" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4654,22 +4654,22 @@
         <v>147</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F140" s="0" t="n">
-        <v>1</v>
+        <v>280</v>
       </c>
       <c r="G140" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H140" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I140" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4683,16 +4683,16 @@
         <v>147</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="F141" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G141" s="0" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="H141" s="0" t="s">
         <v>13</v>
@@ -4712,16 +4712,16 @@
         <v>147</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G142" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="H142" s="0" t="s">
         <v>13</v>
@@ -4741,13 +4741,13 @@
         <v>147</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E143" s="0" t="s">
         <v>139</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G143" s="0" t="s">
         <v>16</v>
@@ -4770,22 +4770,22 @@
         <v>147</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E144" s="0" t="s">
         <v>140</v>
       </c>
       <c r="F144" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G144" s="0" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="H144" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I144" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4799,7 +4799,7 @@
         <v>147</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E145" s="0" t="s">
         <v>141</v>
@@ -4808,7 +4808,7 @@
         <v>1</v>
       </c>
       <c r="G145" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H145" s="0" t="s">
         <v>13</v>
@@ -4828,22 +4828,22 @@
         <v>147</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="G146" s="0" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="H146" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I146" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4857,22 +4857,22 @@
         <v>147</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>5</v>
+        <v>300</v>
       </c>
       <c r="G147" s="0" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="H147" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I147" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4886,22 +4886,22 @@
         <v>147</v>
       </c>
       <c r="D148" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E148" s="0" t="s">
-        <v>142</v>
+        <v>18</v>
       </c>
       <c r="F148" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G148" s="0" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="H148" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I148" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4912,16 +4912,16 @@
         <v>78</v>
       </c>
       <c r="C149" s="0" t="n">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D149" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E149" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="E149" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="F149" s="0" t="n">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G149" s="0" t="s">
         <v>16</v>
@@ -4930,7 +4930,7 @@
         <v>13</v>
       </c>
       <c r="I149" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4944,13 +4944,13 @@
         <v>148</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E150" s="0" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>30</v>
+        <v>280</v>
       </c>
       <c r="G150" s="0" t="s">
         <v>16</v>
@@ -4959,7 +4959,7 @@
         <v>13</v>
       </c>
       <c r="I150" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4973,16 +4973,16 @@
         <v>148</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E151" s="0" t="s">
         <v>145</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G151" s="0" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="H151" s="0" t="s">
         <v>13</v>
@@ -5002,22 +5002,22 @@
         <v>148</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="F152" s="0" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="G152" s="0" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="H152" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I152" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5031,16 +5031,16 @@
         <v>148</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E153" s="0" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="F153" s="0" t="n">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="G153" s="0" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="H153" s="0" t="s">
         <v>13</v>
@@ -5060,22 +5060,22 @@
         <v>148</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>15</v>
+        <v>147</v>
       </c>
       <c r="F154" s="0" t="n">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="G154" s="0" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="H154" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I154" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5089,13 +5089,13 @@
         <v>148</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>97</v>
+        <v>15</v>
       </c>
       <c r="F155" s="0" t="n">
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="G155" s="0" t="s">
         <v>16</v>
@@ -5104,7 +5104,7 @@
         <v>13</v>
       </c>
       <c r="I155" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5118,22 +5118,22 @@
         <v>148</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F156" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="G156" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H156" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I156" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5141,28 +5141,28 @@
         <v>9</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C157" s="0" t="n">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E157" s="0" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="F157" s="0" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G157" s="0" t="s">
         <v>12</v>
       </c>
       <c r="H157" s="0" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="I157" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5176,22 +5176,22 @@
         <v>98</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E158" s="0" t="s">
         <v>149</v>
       </c>
       <c r="F158" s="0" t="n">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="G158" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H158" s="0" t="s">
         <v>81</v>
       </c>
       <c r="I158" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5205,22 +5205,22 @@
         <v>98</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E159" s="0" t="s">
         <v>150</v>
       </c>
       <c r="F159" s="0" t="n">
-        <v>80</v>
+        <v>400</v>
       </c>
       <c r="G159" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H159" s="0" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="I159" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,13 +5234,13 @@
         <v>98</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E160" s="0" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
       <c r="F160" s="0" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="G160" s="0" t="s">
         <v>16</v>
@@ -5252,8 +5252,37 @@
         <v>24</v>
       </c>
     </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="D161" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E161" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F161" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G161" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H161" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I161" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H160"/>
+  <autoFilter ref="A1:H161"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>